<commit_message>
Implement sync of Table entities between Actual and Archive.
</commit_message>
<xml_diff>
--- a/design/doc/entity_storage.xlsx
+++ b/design/doc/entity_storage.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\git\Receipt\design\doc\"/>
@@ -118,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +131,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -261,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -269,9 +281,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,7 +573,7 @@
   <dimension ref="D3:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H9" sqref="H9:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,16 +600,16 @@
       </c>
     </row>
     <row r="5" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6"/>
+      <c r="F5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4" t="s">
@@ -608,16 +626,16 @@
       </c>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="6"/>
+      <c r="F7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
@@ -679,64 +697,64 @@
       </c>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="6"/>
+      <c r="F12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="6"/>
+      <c r="F13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="6"/>
+      <c r="F14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="9"/>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="6"/>
+      <c r="F15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="6"/>
+      <c r="F16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
@@ -751,16 +769,16 @@
       <c r="G17" s="6"/>
     </row>
     <row r="18" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>